<commit_message>
Actualización modelo información planilla
</commit_message>
<xml_diff>
--- a/django_project_pss/media/datos_entidades.xlsx
+++ b/django_project_pss/media/datos_entidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naguie\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11815EBA-34F4-4690-8C03-54226178BBFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508F6B0B-0F37-4476-A7E5-09B93C2C9B7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -367,42 +367,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -584,6 +548,42 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -598,25 +598,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03A52D7A-920D-466D-B3F0-D1D11F5586E6}" name="Tabla1" displayName="Tabla1" ref="A1:J27" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:J27" xr:uid="{7E14A0BE-40E9-4A55-91F6-37A47E2DE503}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="899999034"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03A52D7A-920D-466D-B3F0-D1D11F5586E6}" name="Tabla1" displayName="Tabla1" ref="A1:J27" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J27" xr:uid="{7E14A0BE-40E9-4A55-91F6-37A47E2DE503}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CF978527-F7BA-4B9B-B8AD-1274DEA2A744}" name="NIT" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{0E67C83E-2715-4004-9CF0-E0E1E86AC6AE}" name="codigo" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{915A7CCD-F921-4E1C-ACD7-F26931D4BA7C}" name="idTipoGasto" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{D8E626CF-42C3-4F41-93A0-524A9EEA5F22}" name="concepto" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{3D4FAFEF-18EC-41F2-BF31-3046A91B9B25}" name="razonEntidad" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{9E09FEED-97DC-4011-8072-97915BD69386}" name="rubroPermanente" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{5F925F29-CA5F-48BD-A949-62C8EA11636D}" name="rubroTemporal" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{54A37354-64CE-4AC8-970A-45D26A86742C}" name="tipoCuentaPagar" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{45470127-6737-421F-BA9D-05ACC650B491}" name="codigoDescuento" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{8C3B5071-35FA-4655-A501-F151EE8A4C20}" name="tipo" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{CF978527-F7BA-4B9B-B8AD-1274DEA2A744}" name="NIT" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{0E67C83E-2715-4004-9CF0-E0E1E86AC6AE}" name="codigo" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{915A7CCD-F921-4E1C-ACD7-F26931D4BA7C}" name="idTipoGasto" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{D8E626CF-42C3-4F41-93A0-524A9EEA5F22}" name="concepto" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{3D4FAFEF-18EC-41F2-BF31-3046A91B9B25}" name="razonEntidad" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{9E09FEED-97DC-4011-8072-97915BD69386}" name="rubroPermanente" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{5F925F29-CA5F-48BD-A949-62C8EA11636D}" name="rubroTemporal" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{54A37354-64CE-4AC8-970A-45D26A86742C}" name="tipoCuentaPagar" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{45470127-6737-421F-BA9D-05ACC650B491}" name="codigoDescuento" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{8C3B5071-35FA-4655-A501-F151EE8A4C20}" name="tipo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -936,7 +930,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>800088702</v>
       </c>
@@ -968,7 +962,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>805001157</v>
       </c>
@@ -1000,7 +994,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>800130907</v>
       </c>
@@ -1032,7 +1026,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>800251440</v>
       </c>
@@ -1064,7 +1058,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>900156264</v>
       </c>
@@ -1096,7 +1090,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>809008362</v>
       </c>
@@ -1128,7 +1122,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>900935126</v>
       </c>
@@ -1160,7 +1154,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>860066942</v>
       </c>
@@ -1192,7 +1186,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>890303093</v>
       </c>
@@ -1224,7 +1218,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>830003564</v>
       </c>
@@ -1256,7 +1250,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>901037916</v>
       </c>
@@ -1288,7 +1282,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>900226715</v>
       </c>
@@ -1320,7 +1314,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>900336004</v>
       </c>
@@ -1352,7 +1346,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>800229739</v>
       </c>
@@ -1384,7 +1378,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>800227940</v>
       </c>
@@ -1416,7 +1410,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>800224808</v>
       </c>
@@ -1448,7 +1442,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>860011153</v>
       </c>
@@ -1480,7 +1474,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>891480000</v>
       </c>
@@ -1512,7 +1506,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>899999239</v>
       </c>
@@ -1576,7 +1570,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>899999054</v>
       </c>
@@ -1608,7 +1602,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>899999001</v>
       </c>
@@ -1640,7 +1634,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>901097473</v>
       </c>
@@ -1672,7 +1666,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>805000427</v>
       </c>
@@ -1704,7 +1698,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>814000337</v>
       </c>
@@ -1736,7 +1730,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>800140949</v>
       </c>

</xml_diff>

<commit_message>
Cambios en datos entidades para que funcione con el nuevo formato
</commit_message>
<xml_diff>
--- a/django_project_pss/media/datos_entidades.xlsx
+++ b/django_project_pss/media/datos_entidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naguie\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508F6B0B-0F37-4476-A7E5-09B93C2C9B7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6926E41C-DCDE-41AF-B79A-240DDC7DC550}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -882,7 +882,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1517,10 +1517,10 @@
         <v>26</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>21</v>
@@ -1581,10 +1581,10 @@
         <v>26</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>23</v>

</xml_diff>